<commit_message>
Add survey instructions, update files
</commit_message>
<xml_diff>
--- a/statistics_files/2022/99.year.end/2022.state.survey.xlsx
+++ b/statistics_files/2022/99.year.end/2022.state.survey.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Linked in NEXT\Statistics\2021\next\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\GitHub\next_statistics\statistics_files\2022\99.year.end\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7B64733-1665-48E2-84E5-20F6CE959D14}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{386C33CD-1681-485F-85D8-97AEC7737781}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,14 +26,14 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'State Survey-2019 data'!$A$1:$N$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'State Survey-2020 data'!$A$1:$N$57</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'State Survey-2021 data'!$A$1:$M$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'State Survey-2022 data'!$A$1:$M$57</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'State Survey-2022 data'!$A$1:$M$55</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="163">
   <si>
     <t>branchcode</t>
   </si>
@@ -354,6 +354,177 @@
   <si>
     <t>Question 11.4 - circulation "Other physical items"</t>
   </si>
+  <si>
+    <t>Atchison Public Library</t>
+  </si>
+  <si>
+    <t>Baldwin City Public Library</t>
+  </si>
+  <si>
+    <t>Basehor Community Library</t>
+  </si>
+  <si>
+    <t>Bern Community Library</t>
+  </si>
+  <si>
+    <t>Bonner Springs City Library</t>
+  </si>
+  <si>
+    <t>Burlingame Community Library</t>
+  </si>
+  <si>
+    <t>Carbondale City Library</t>
+  </si>
+  <si>
+    <t>Centralia Community Library</t>
+  </si>
+  <si>
+    <t>Corning City Library</t>
+  </si>
+  <si>
+    <t>Digital Content</t>
+  </si>
+  <si>
+    <t>Doniphan County Library - Elwood</t>
+  </si>
+  <si>
+    <t>Doniphan County Library - Highland</t>
+  </si>
+  <si>
+    <t>Doniphan County Library - Troy</t>
+  </si>
+  <si>
+    <t>Doniphan County Library - Wathena</t>
+  </si>
+  <si>
+    <t>Effingham Community Library</t>
+  </si>
+  <si>
+    <t>Eudora Community Library</t>
+  </si>
+  <si>
+    <t>Everest, Barnes Reading Room</t>
+  </si>
+  <si>
+    <t>Hiawatha, Morrill Public Library</t>
+  </si>
+  <si>
+    <t>Highland Community College</t>
+  </si>
+  <si>
+    <t>Holton, Beck-Bookman Library</t>
+  </si>
+  <si>
+    <t>Horton Public Library</t>
+  </si>
+  <si>
+    <t>Lansing Community Library</t>
+  </si>
+  <si>
+    <t>Leavenworth Public Library</t>
+  </si>
+  <si>
+    <t>Linwood Community Library</t>
+  </si>
+  <si>
+    <t>Louisburg Library</t>
+  </si>
+  <si>
+    <t>Lyndon Carnegie Library</t>
+  </si>
+  <si>
+    <t>McLouth Public Library</t>
+  </si>
+  <si>
+    <t>Meriden-Ozawkie Public Library</t>
+  </si>
+  <si>
+    <t>Northeast Kansas Library System</t>
+  </si>
+  <si>
+    <t>Nortonville Public Library</t>
+  </si>
+  <si>
+    <t>Osage City Library</t>
+  </si>
+  <si>
+    <t>Osawatomie Public Library</t>
+  </si>
+  <si>
+    <t>Oskaloosa Public Library</t>
+  </si>
+  <si>
+    <t>Ottawa Library</t>
+  </si>
+  <si>
+    <t>Overbrook Public Library</t>
+  </si>
+  <si>
+    <t>Paola Free Library</t>
+  </si>
+  <si>
+    <t>Perry-Lecompton Community Library</t>
+  </si>
+  <si>
+    <t>Pomona Community Library</t>
+  </si>
+  <si>
+    <t>Prairie Hills Schools - Axtell Public School</t>
+  </si>
+  <si>
+    <t>Prairie Hills Schools - Sabetha Elementary School</t>
+  </si>
+  <si>
+    <t>Prairie Hills Schools - Sabetha High School</t>
+  </si>
+  <si>
+    <t>Prairie Hills Schools - Sabetha Middle School</t>
+  </si>
+  <si>
+    <t>Prairie Hills Schools - Wetmore Academic Center</t>
+  </si>
+  <si>
+    <t>Richmond Public Library</t>
+  </si>
+  <si>
+    <t>Rossville Community Library</t>
+  </si>
+  <si>
+    <t>Sabetha, Mary Cotton Library</t>
+  </si>
+  <si>
+    <t>Seneca Free Library</t>
+  </si>
+  <si>
+    <t>Silver Lake Library</t>
+  </si>
+  <si>
+    <t>Tonganoxie Public Library</t>
+  </si>
+  <si>
+    <t>Valley Falls, Delaware Township Library</t>
+  </si>
+  <si>
+    <t>Wellsville City Library</t>
+  </si>
+  <si>
+    <t>Wetmore Public Library</t>
+  </si>
+  <si>
+    <t>Williamsburg Community Library</t>
+  </si>
+  <si>
+    <t>Winchester Public Library</t>
+  </si>
+  <si>
+    <t>Doniphan County - All</t>
+  </si>
+  <si>
+    <t>Prairie Hills School District - All</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
 </sst>
 </file>
 
@@ -502,7 +673,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="40">
+  <fills count="42">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -724,6 +895,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -907,7 +1090,7 @@
     <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -953,6 +1136,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="39" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1287,7 +1479,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D96722BF-9183-4139-AEEB-D79FB90E8DE7}">
-  <dimension ref="A1:M57"/>
+  <dimension ref="A1:M58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -1298,7 +1490,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="13" width="16.7109375" style="7" customWidth="1"/>
+    <col min="1" max="1" width="44.7109375" style="7" customWidth="1"/>
+    <col min="2" max="13" width="16.7109375" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="9" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1343,1042 +1536,2396 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="1">
+        <v>6386</v>
+      </c>
+      <c r="C2" s="1">
+        <v>49570</v>
+      </c>
+      <c r="D2" s="1">
+        <v>3077</v>
+      </c>
+      <c r="E2" s="1">
+        <v>3677</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2470</v>
+      </c>
+      <c r="G2" s="1">
+        <v>5934</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1340</v>
+      </c>
+      <c r="I2" s="1">
+        <v>34429</v>
+      </c>
+      <c r="J2" s="1">
+        <v>37031</v>
+      </c>
+      <c r="K2" s="15">
+        <v>1462</v>
+      </c>
+      <c r="L2" s="1">
+        <v>10860</v>
+      </c>
+      <c r="M2" s="1">
+        <v>11578</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" s="2">
+        <v>3857</v>
+      </c>
+      <c r="C3" s="2">
+        <v>22570</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1291</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1919</v>
+      </c>
+      <c r="F3" s="2">
+        <v>562</v>
+      </c>
+      <c r="G3" s="2">
+        <v>2860</v>
+      </c>
+      <c r="H3" s="2">
+        <v>603</v>
+      </c>
+      <c r="I3" s="2">
+        <v>15036</v>
+      </c>
+      <c r="J3" s="2">
+        <v>18825</v>
+      </c>
+      <c r="K3" s="16">
+        <v>1127</v>
+      </c>
+      <c r="L3" s="2">
+        <v>4036</v>
+      </c>
+      <c r="M3" s="2">
+        <v>4091</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4" s="1">
+        <v>6361</v>
+      </c>
+      <c r="C4" s="1">
+        <v>53196</v>
+      </c>
+      <c r="D4" s="1">
+        <v>4178</v>
+      </c>
+      <c r="E4" s="1">
+        <v>4829</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2382</v>
+      </c>
+      <c r="G4" s="1">
+        <v>7936</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1165</v>
+      </c>
+      <c r="I4" s="1">
+        <v>48424</v>
+      </c>
+      <c r="J4" s="1">
+        <v>70073</v>
+      </c>
+      <c r="K4" s="15">
+        <v>3814</v>
+      </c>
+      <c r="L4" s="1">
+        <v>8844</v>
+      </c>
+      <c r="M4" s="1">
+        <v>11315</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" s="2">
+        <v>174</v>
+      </c>
+      <c r="C5" s="2">
+        <v>10027</v>
+      </c>
+      <c r="D5" s="2">
+        <v>259</v>
+      </c>
+      <c r="E5" s="2">
+        <v>50</v>
+      </c>
+      <c r="F5" s="2">
+        <v>811</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1322</v>
+      </c>
+      <c r="H5" s="2">
+        <v>83</v>
+      </c>
+      <c r="I5" s="2">
+        <v>1176</v>
+      </c>
+      <c r="J5" s="2">
+        <v>1263</v>
+      </c>
+      <c r="K5" s="16">
         <v>1</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="L5" s="2">
+        <v>824</v>
+      </c>
+      <c r="M5" s="2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6" s="1">
+        <v>8030</v>
+      </c>
+      <c r="C6" s="1">
+        <v>48813</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3956</v>
+      </c>
+      <c r="E6" s="1">
+        <v>3079</v>
+      </c>
+      <c r="F6" s="1">
+        <v>3356</v>
+      </c>
+      <c r="G6" s="1">
+        <v>5640</v>
+      </c>
+      <c r="H6" s="1">
+        <v>2009</v>
+      </c>
+      <c r="I6" s="1">
+        <v>29178</v>
+      </c>
+      <c r="J6" s="1">
+        <v>40691</v>
+      </c>
+      <c r="K6" s="15">
+        <v>3201</v>
+      </c>
+      <c r="L6" s="1">
+        <v>12493</v>
+      </c>
+      <c r="M6" s="1">
+        <v>10946</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7" s="2">
+        <v>634</v>
+      </c>
+      <c r="C7" s="2">
+        <v>10982</v>
+      </c>
+      <c r="D7" s="2">
+        <v>420</v>
+      </c>
+      <c r="E7" s="2">
+        <v>777</v>
+      </c>
+      <c r="F7" s="2">
+        <v>685</v>
+      </c>
+      <c r="G7" s="2">
+        <v>2963</v>
+      </c>
+      <c r="H7" s="2">
+        <v>216</v>
+      </c>
+      <c r="I7" s="2">
+        <v>4785</v>
+      </c>
+      <c r="J7" s="2">
+        <v>2891</v>
+      </c>
+      <c r="K7" s="16">
+        <v>1334</v>
+      </c>
+      <c r="L7" s="2">
+        <v>1934</v>
+      </c>
+      <c r="M7" s="2">
+        <v>1755</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="B8" s="1">
+        <v>731</v>
+      </c>
+      <c r="C8" s="1">
+        <v>7078</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2146</v>
+      </c>
+      <c r="E8" s="1">
+        <v>611</v>
+      </c>
+      <c r="F8" s="1">
+        <v>7</v>
+      </c>
+      <c r="G8" s="1">
+        <v>2365</v>
+      </c>
+      <c r="H8" s="1">
+        <v>36</v>
+      </c>
+      <c r="I8" s="1">
+        <v>5938</v>
+      </c>
+      <c r="J8" s="1">
+        <v>3310</v>
+      </c>
+      <c r="K8" s="15">
+        <v>54</v>
+      </c>
+      <c r="L8" s="1">
+        <v>1674</v>
+      </c>
+      <c r="M8" s="1">
+        <v>1172</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="B9" s="2">
+        <v>238</v>
+      </c>
+      <c r="C9" s="2">
+        <v>6667</v>
+      </c>
+      <c r="D9" s="2">
+        <v>474</v>
+      </c>
+      <c r="E9" s="2">
+        <v>158</v>
+      </c>
+      <c r="F9" s="2">
+        <v>322</v>
+      </c>
+      <c r="G9" s="2">
+        <v>767</v>
+      </c>
+      <c r="H9" s="2">
+        <v>42</v>
+      </c>
+      <c r="I9" s="2">
+        <v>2189</v>
+      </c>
+      <c r="J9" s="2">
+        <v>1271</v>
+      </c>
+      <c r="K9" s="16">
+        <v>18</v>
+      </c>
+      <c r="L9" s="2">
+        <v>601</v>
+      </c>
+      <c r="M9" s="2">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="B10" s="1">
+        <v>149</v>
+      </c>
+      <c r="C10" s="1">
+        <v>4516</v>
+      </c>
+      <c r="D10" s="1">
+        <v>223</v>
+      </c>
+      <c r="E10" s="1">
+        <v>141</v>
+      </c>
+      <c r="F10" s="1">
+        <v>57</v>
+      </c>
+      <c r="G10" s="1">
+        <v>595</v>
+      </c>
+      <c r="H10" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="I10" s="1">
+        <v>142</v>
+      </c>
+      <c r="J10" s="1">
+        <v>331</v>
+      </c>
+      <c r="K10" s="15">
+        <v>0</v>
+      </c>
+      <c r="L10" s="1">
+        <v>418</v>
+      </c>
+      <c r="M10" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="B11" s="2">
+        <v>55</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0</v>
+      </c>
+      <c r="H11" s="2">
+        <v>361</v>
+      </c>
+      <c r="I11" s="2">
+        <v>0</v>
+      </c>
+      <c r="J11" s="2">
+        <v>0</v>
+      </c>
+      <c r="K11" s="16">
+        <v>0</v>
+      </c>
+      <c r="L11" s="2">
+        <v>0</v>
+      </c>
+      <c r="M11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="B12" s="3">
+        <v>399</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1313</v>
+      </c>
+      <c r="D12" s="3">
+        <v>194</v>
+      </c>
+      <c r="E12" s="3">
+        <v>153</v>
+      </c>
+      <c r="F12" s="3">
+        <v>87</v>
+      </c>
+      <c r="G12" s="3">
+        <v>1205</v>
+      </c>
+      <c r="H12" s="3">
+        <v>105</v>
+      </c>
+      <c r="I12" s="3">
+        <v>760</v>
+      </c>
+      <c r="J12" s="3">
+        <v>473</v>
+      </c>
+      <c r="K12" s="17">
+        <v>378</v>
+      </c>
+      <c r="L12" s="3">
+        <v>463</v>
+      </c>
+      <c r="M12" s="3">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="B13" s="3">
+        <v>383</v>
+      </c>
+      <c r="C13" s="3">
+        <v>3259</v>
+      </c>
+      <c r="D13" s="3">
+        <v>370</v>
+      </c>
+      <c r="E13" s="3">
+        <v>785</v>
+      </c>
+      <c r="F13" s="3">
+        <v>75</v>
+      </c>
+      <c r="G13" s="3">
+        <v>1221</v>
+      </c>
+      <c r="H13" s="3">
+        <v>214</v>
+      </c>
+      <c r="I13" s="3">
+        <v>3004</v>
+      </c>
+      <c r="J13" s="3">
+        <v>1500</v>
+      </c>
+      <c r="K13" s="17">
+        <v>669</v>
+      </c>
+      <c r="L13" s="3">
+        <v>2133</v>
+      </c>
+      <c r="M13" s="3">
+        <v>1601</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="B14" s="3">
+        <v>919</v>
+      </c>
+      <c r="C14" s="3">
+        <v>9398</v>
+      </c>
+      <c r="D14" s="3">
+        <v>968</v>
+      </c>
+      <c r="E14" s="3">
+        <v>898</v>
+      </c>
+      <c r="F14" s="3">
+        <v>279</v>
+      </c>
+      <c r="G14" s="3">
+        <v>1429</v>
+      </c>
+      <c r="H14" s="3">
+        <v>257</v>
+      </c>
+      <c r="I14" s="3">
+        <v>5206</v>
+      </c>
+      <c r="J14" s="3">
+        <v>4216</v>
+      </c>
+      <c r="K14" s="17">
+        <v>627</v>
+      </c>
+      <c r="L14" s="3">
+        <v>3316</v>
+      </c>
+      <c r="M14" s="3">
+        <v>1454</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="B15" s="3">
+        <v>562</v>
+      </c>
+      <c r="C15" s="3">
+        <v>5402</v>
+      </c>
+      <c r="D15" s="3">
+        <v>743</v>
+      </c>
+      <c r="E15" s="3">
+        <v>593</v>
+      </c>
+      <c r="F15" s="3">
+        <v>233</v>
+      </c>
+      <c r="G15" s="3">
+        <v>1792</v>
+      </c>
+      <c r="H15" s="3">
+        <v>176</v>
+      </c>
+      <c r="I15" s="3">
+        <v>2725</v>
+      </c>
+      <c r="J15" s="3">
+        <v>2499</v>
+      </c>
+      <c r="K15" s="17">
+        <v>352</v>
+      </c>
+      <c r="L15" s="3">
+        <v>2303</v>
+      </c>
+      <c r="M15" s="3">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="B16" s="2">
+        <v>330</v>
+      </c>
+      <c r="C16" s="2">
+        <v>7565</v>
+      </c>
+      <c r="D16" s="2">
+        <v>489</v>
+      </c>
+      <c r="E16" s="2">
+        <v>308</v>
+      </c>
+      <c r="F16" s="2">
+        <v>66</v>
+      </c>
+      <c r="G16" s="2">
+        <v>799</v>
+      </c>
+      <c r="H16" s="2">
+        <v>13</v>
+      </c>
+      <c r="I16" s="2">
+        <v>1575</v>
+      </c>
+      <c r="J16" s="2">
+        <v>1700</v>
+      </c>
+      <c r="K16" s="16">
+        <v>18</v>
+      </c>
+      <c r="L16" s="2">
+        <v>1147</v>
+      </c>
+      <c r="M16" s="2">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1826</v>
+      </c>
+      <c r="C17" s="1">
+        <v>13709</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1136</v>
+      </c>
+      <c r="E17" s="1">
+        <v>665</v>
+      </c>
+      <c r="F17" s="1">
+        <v>659</v>
+      </c>
+      <c r="G17" s="1">
+        <v>1628</v>
+      </c>
+      <c r="H17" s="1">
+        <v>70</v>
+      </c>
+      <c r="I17" s="1">
+        <v>9370</v>
+      </c>
+      <c r="J17" s="1">
+        <v>17800</v>
+      </c>
+      <c r="K17" s="15">
+        <v>332</v>
+      </c>
+      <c r="L17" s="1">
+        <v>4312</v>
+      </c>
+      <c r="M17" s="1">
+        <v>5134</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="B18" s="2">
+        <v>144</v>
+      </c>
+      <c r="C18" s="2">
+        <v>10478</v>
+      </c>
+      <c r="D18" s="2">
+        <v>507</v>
+      </c>
+      <c r="E18" s="2">
+        <v>58</v>
+      </c>
+      <c r="F18" s="2">
+        <v>116</v>
+      </c>
+      <c r="G18" s="2">
+        <v>1395</v>
+      </c>
+      <c r="H18" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="I18" s="2">
+        <v>1993</v>
+      </c>
+      <c r="J18" s="2">
+        <v>2720</v>
+      </c>
+      <c r="K18" s="16">
+        <v>8</v>
+      </c>
+      <c r="L18" s="2">
+        <v>1190</v>
+      </c>
+      <c r="M18" s="2">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="B19" s="1">
+        <v>2541</v>
+      </c>
+      <c r="C19" s="1">
+        <v>27478</v>
+      </c>
+      <c r="D19" s="1">
+        <v>998</v>
+      </c>
+      <c r="E19" s="1">
+        <v>670</v>
+      </c>
+      <c r="F19" s="1">
+        <v>727</v>
+      </c>
+      <c r="G19" s="1">
+        <v>1793</v>
+      </c>
+      <c r="H19" s="1">
+        <v>394</v>
+      </c>
+      <c r="I19" s="1">
+        <v>15047</v>
+      </c>
+      <c r="J19" s="1">
+        <v>18840</v>
+      </c>
+      <c r="K19" s="15">
+        <v>330</v>
+      </c>
+      <c r="L19" s="1">
+        <v>3754</v>
+      </c>
+      <c r="M19" s="1">
+        <v>5965</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="B20" s="2">
+        <v>9230</v>
+      </c>
+      <c r="C20" s="2">
+        <v>3956</v>
+      </c>
+      <c r="D20" s="2">
+        <v>244</v>
+      </c>
+      <c r="E20" s="2">
+        <v>929</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0</v>
+      </c>
+      <c r="G20" s="2">
+        <v>443</v>
+      </c>
+      <c r="H20" s="2">
+        <v>689</v>
+      </c>
+      <c r="I20" s="2">
+        <v>437</v>
+      </c>
+      <c r="J20" s="2">
+        <v>72</v>
+      </c>
+      <c r="K20" s="16">
+        <v>207</v>
+      </c>
+      <c r="L20" s="2">
+        <v>523</v>
+      </c>
+      <c r="M20" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="B21" s="1">
+        <v>3987</v>
+      </c>
+      <c r="C21" s="1">
+        <v>22768</v>
+      </c>
+      <c r="D21" s="1">
+        <v>955</v>
+      </c>
+      <c r="E21" s="1">
+        <v>2324</v>
+      </c>
+      <c r="F21" s="1">
+        <v>938</v>
+      </c>
+      <c r="G21" s="1">
+        <v>2460</v>
+      </c>
+      <c r="H21" s="1">
+        <v>691</v>
+      </c>
+      <c r="I21" s="1">
+        <v>16641</v>
+      </c>
+      <c r="J21" s="1">
+        <v>11614</v>
+      </c>
+      <c r="K21" s="15">
+        <v>553</v>
+      </c>
+      <c r="L21" s="1">
+        <v>3522</v>
+      </c>
+      <c r="M21" s="1">
+        <v>4674</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B22" s="2">
+        <v>1180</v>
+      </c>
+      <c r="C22" s="2">
+        <v>11383</v>
+      </c>
+      <c r="D22" s="2">
+        <v>284</v>
+      </c>
+      <c r="E22" s="2">
+        <v>160</v>
+      </c>
+      <c r="F22" s="2">
+        <v>424</v>
+      </c>
+      <c r="G22" s="2">
+        <v>1789</v>
+      </c>
+      <c r="H22" s="2">
+        <v>539</v>
+      </c>
+      <c r="I22" s="2">
+        <v>1331</v>
+      </c>
+      <c r="J22" s="2">
+        <v>545</v>
+      </c>
+      <c r="K22" s="16">
+        <v>99</v>
+      </c>
+      <c r="L22" s="2">
+        <v>781</v>
+      </c>
+      <c r="M22" s="2">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="B23" s="1">
+        <v>3096</v>
+      </c>
+      <c r="C23" s="1">
+        <v>17648</v>
+      </c>
+      <c r="D23" s="1">
+        <v>2017</v>
+      </c>
+      <c r="E23" s="1">
+        <v>1375</v>
+      </c>
+      <c r="F23" s="1">
+        <v>461</v>
+      </c>
+      <c r="G23" s="1">
+        <v>3662</v>
+      </c>
+      <c r="H23" s="1">
+        <v>517</v>
+      </c>
+      <c r="I23" s="1">
+        <v>12421</v>
+      </c>
+      <c r="J23" s="1">
+        <v>16763</v>
+      </c>
+      <c r="K23" s="15">
+        <v>862</v>
+      </c>
+      <c r="L23" s="1">
+        <v>5162</v>
+      </c>
+      <c r="M23" s="1">
+        <v>5263</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="B24" s="2">
+        <v>14308</v>
+      </c>
+      <c r="C24" s="2">
+        <v>69014</v>
+      </c>
+      <c r="D24" s="2">
+        <v>4874</v>
+      </c>
+      <c r="E24" s="2">
+        <v>8221</v>
+      </c>
+      <c r="F24" s="2">
+        <v>6077</v>
+      </c>
+      <c r="G24" s="2">
+        <v>10507</v>
+      </c>
+      <c r="H24" s="2">
+        <v>6038</v>
+      </c>
+      <c r="I24" s="2">
+        <v>54804</v>
+      </c>
+      <c r="J24" s="2">
+        <v>57294</v>
+      </c>
+      <c r="K24" s="16">
+        <v>4500</v>
+      </c>
+      <c r="L24" s="2">
+        <v>12922</v>
+      </c>
+      <c r="M24" s="2">
+        <v>12989</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="B25" s="1">
+        <v>631</v>
+      </c>
+      <c r="C25" s="1">
+        <v>9697</v>
+      </c>
+      <c r="D25" s="1">
+        <v>837</v>
+      </c>
+      <c r="E25" s="1">
+        <v>1425</v>
+      </c>
+      <c r="F25" s="1">
+        <v>274</v>
+      </c>
+      <c r="G25" s="1">
+        <v>2306</v>
+      </c>
+      <c r="H25" s="1">
+        <v>316</v>
+      </c>
+      <c r="I25" s="1">
+        <v>3636</v>
+      </c>
+      <c r="J25" s="1">
+        <v>4367</v>
+      </c>
+      <c r="K25" s="15">
+        <v>421</v>
+      </c>
+      <c r="L25" s="1">
+        <v>3058</v>
+      </c>
+      <c r="M25" s="1">
+        <v>1173</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="B26" s="2">
+        <v>578</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0</v>
+      </c>
+      <c r="F26" s="2">
+        <v>0</v>
+      </c>
+      <c r="G26" s="2">
+        <v>0</v>
+      </c>
+      <c r="H26" s="2">
+        <v>0</v>
+      </c>
+      <c r="I26" s="2">
+        <v>0</v>
+      </c>
+      <c r="J26" s="2">
+        <v>0</v>
+      </c>
+      <c r="K26" s="16">
+        <v>0</v>
+      </c>
+      <c r="L26" s="2">
+        <v>0</v>
+      </c>
+      <c r="M26" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="B27" s="1">
+        <v>971</v>
+      </c>
+      <c r="C27" s="1">
+        <v>11537</v>
+      </c>
+      <c r="D27" s="1">
+        <v>868</v>
+      </c>
+      <c r="E27" s="1">
+        <v>1312</v>
+      </c>
+      <c r="F27" s="1">
+        <v>475</v>
+      </c>
+      <c r="G27" s="1">
+        <v>2054</v>
+      </c>
+      <c r="H27" s="1">
+        <v>156</v>
+      </c>
+      <c r="I27" s="1">
+        <v>5884</v>
+      </c>
+      <c r="J27" s="1">
+        <v>3509</v>
+      </c>
+      <c r="K27" s="15">
+        <v>183</v>
+      </c>
+      <c r="L27" s="1">
+        <v>1899</v>
+      </c>
+      <c r="M27" s="1">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="B28" s="2">
+        <v>584</v>
+      </c>
+      <c r="C28" s="2">
+        <v>3118</v>
+      </c>
+      <c r="D28" s="2">
+        <v>378</v>
+      </c>
+      <c r="E28" s="2">
+        <v>253</v>
+      </c>
+      <c r="F28" s="2">
+        <v>22</v>
+      </c>
+      <c r="G28" s="2">
+        <v>592</v>
+      </c>
+      <c r="H28" s="2">
+        <v>48</v>
+      </c>
+      <c r="I28" s="2">
+        <v>1313</v>
+      </c>
+      <c r="J28" s="2">
+        <v>2254</v>
+      </c>
+      <c r="K28" s="16">
+        <v>15</v>
+      </c>
+      <c r="L28" s="2">
+        <v>573</v>
+      </c>
+      <c r="M28" s="2">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="B29" s="1">
+        <v>1678</v>
+      </c>
+      <c r="C29" s="1">
+        <v>13188</v>
+      </c>
+      <c r="D29" s="1">
+        <v>1440</v>
+      </c>
+      <c r="E29" s="1">
+        <v>1550</v>
+      </c>
+      <c r="F29" s="1">
+        <v>560</v>
+      </c>
+      <c r="G29" s="1">
+        <v>2419</v>
+      </c>
+      <c r="H29" s="1">
+        <v>98</v>
+      </c>
+      <c r="I29" s="1">
+        <v>10626</v>
+      </c>
+      <c r="J29" s="1">
+        <v>15092</v>
+      </c>
+      <c r="K29" s="15">
+        <v>471</v>
+      </c>
+      <c r="L29" s="1">
+        <v>4777</v>
+      </c>
+      <c r="M29" s="1">
+        <v>4837</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="B30" s="2">
+        <v>340</v>
+      </c>
+      <c r="C30" s="2">
+        <v>326</v>
+      </c>
+      <c r="D30" s="2">
+        <v>104</v>
+      </c>
+      <c r="E30" s="2">
+        <v>48</v>
+      </c>
+      <c r="F30" s="2">
+        <v>18</v>
+      </c>
+      <c r="G30" s="2">
+        <v>23</v>
+      </c>
+      <c r="H30" s="2">
+        <v>310</v>
+      </c>
+      <c r="I30" s="2">
+        <v>665</v>
+      </c>
+      <c r="J30" s="2">
+        <v>228</v>
+      </c>
+      <c r="K30" s="16">
+        <v>56</v>
+      </c>
+      <c r="L30" s="2">
+        <v>335</v>
+      </c>
+      <c r="M30" s="2">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="B31" s="1">
+        <v>510</v>
+      </c>
+      <c r="C31" s="1">
+        <v>14017</v>
+      </c>
+      <c r="D31" s="1">
+        <v>913</v>
+      </c>
+      <c r="E31" s="1">
+        <v>1787</v>
+      </c>
+      <c r="F31" s="1">
+        <v>300</v>
+      </c>
+      <c r="G31" s="1">
+        <v>3961</v>
+      </c>
+      <c r="H31" s="1">
+        <v>1042</v>
+      </c>
+      <c r="I31" s="1">
+        <v>1144</v>
+      </c>
+      <c r="J31" s="1">
+        <v>2586</v>
+      </c>
+      <c r="K31" s="15">
+        <v>271</v>
+      </c>
+      <c r="L31" s="1">
+        <v>2596</v>
+      </c>
+      <c r="M31" s="1">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B32" s="2">
+        <v>1961</v>
+      </c>
+      <c r="C32" s="2">
+        <v>17415</v>
+      </c>
+      <c r="D32" s="2">
+        <v>1131</v>
+      </c>
+      <c r="E32" s="2">
+        <v>916</v>
+      </c>
+      <c r="F32" s="2">
+        <v>1603</v>
+      </c>
+      <c r="G32" s="2">
+        <v>3266</v>
+      </c>
+      <c r="H32" s="2">
+        <v>927</v>
+      </c>
+      <c r="I32" s="2">
+        <v>14821</v>
+      </c>
+      <c r="J32" s="2">
+        <v>7510</v>
+      </c>
+      <c r="K32" s="16">
+        <v>2728</v>
+      </c>
+      <c r="L32" s="2">
+        <v>5059</v>
+      </c>
+      <c r="M32" s="2">
+        <v>4669</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="B33" s="1">
+        <v>2697</v>
+      </c>
+      <c r="C33" s="1">
+        <v>14511</v>
+      </c>
+      <c r="D33" s="1">
+        <v>1277</v>
+      </c>
+      <c r="E33" s="1">
+        <v>1327</v>
+      </c>
+      <c r="F33" s="1">
+        <v>490</v>
+      </c>
+      <c r="G33" s="1">
+        <v>2322</v>
+      </c>
+      <c r="H33" s="1">
+        <v>147</v>
+      </c>
+      <c r="I33" s="1">
+        <v>10216</v>
+      </c>
+      <c r="J33" s="1">
+        <v>7330</v>
+      </c>
+      <c r="K33" s="15">
+        <v>113</v>
+      </c>
+      <c r="L33" s="1">
+        <v>4291</v>
+      </c>
+      <c r="M33" s="1">
+        <v>4316</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="B34" s="2">
+        <v>1196</v>
+      </c>
+      <c r="C34" s="2">
+        <v>9048</v>
+      </c>
+      <c r="D34" s="2">
+        <v>414</v>
+      </c>
+      <c r="E34" s="2">
+        <v>291</v>
+      </c>
+      <c r="F34" s="2">
+        <v>502</v>
+      </c>
+      <c r="G34" s="2">
+        <v>822</v>
+      </c>
+      <c r="H34" s="2">
+        <v>174</v>
+      </c>
+      <c r="I34" s="2">
+        <v>5192</v>
+      </c>
+      <c r="J34" s="2">
+        <v>3394</v>
+      </c>
+      <c r="K34" s="16">
+        <v>1984</v>
+      </c>
+      <c r="L34" s="2">
+        <v>1251</v>
+      </c>
+      <c r="M34" s="2">
+        <v>2275</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="B35" s="1">
+        <v>8860</v>
+      </c>
+      <c r="C35" s="1">
+        <v>57803</v>
+      </c>
+      <c r="D35" s="1">
+        <v>5453</v>
+      </c>
+      <c r="E35" s="1">
+        <v>3545</v>
+      </c>
+      <c r="F35" s="1">
+        <v>2208</v>
+      </c>
+      <c r="G35" s="1">
+        <v>5934</v>
+      </c>
+      <c r="H35" s="1">
+        <v>2364</v>
+      </c>
+      <c r="I35" s="1">
+        <v>36533</v>
+      </c>
+      <c r="J35" s="1">
+        <v>48158</v>
+      </c>
+      <c r="K35" s="15">
+        <v>2018</v>
+      </c>
+      <c r="L35" s="1">
+        <v>9481</v>
+      </c>
+      <c r="M35" s="1">
+        <v>8891</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="B36" s="2">
+        <v>1164</v>
+      </c>
+      <c r="C36" s="2">
+        <v>15188</v>
+      </c>
+      <c r="D36" s="2">
+        <v>711</v>
+      </c>
+      <c r="E36" s="2">
+        <v>651</v>
+      </c>
+      <c r="F36" s="2">
+        <v>652</v>
+      </c>
+      <c r="G36" s="2">
+        <v>5085</v>
+      </c>
+      <c r="H36" s="2">
+        <v>845</v>
+      </c>
+      <c r="I36" s="2">
+        <v>8094</v>
+      </c>
+      <c r="J36" s="2">
+        <v>5366</v>
+      </c>
+      <c r="K36" s="16">
+        <v>296</v>
+      </c>
+      <c r="L36" s="2">
+        <v>4348</v>
+      </c>
+      <c r="M36" s="2">
+        <v>2287</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="B37" s="1">
+        <v>5164</v>
+      </c>
+      <c r="C37" s="1">
+        <v>25792</v>
+      </c>
+      <c r="D37" s="1">
+        <v>1563</v>
+      </c>
+      <c r="E37" s="1">
+        <v>2661</v>
+      </c>
+      <c r="F37" s="1">
+        <v>1314</v>
+      </c>
+      <c r="G37" s="1">
+        <v>1648</v>
+      </c>
+      <c r="H37" s="1">
+        <v>2094</v>
+      </c>
+      <c r="I37" s="1">
+        <v>13514</v>
+      </c>
+      <c r="J37" s="1">
+        <v>16358</v>
+      </c>
+      <c r="K37" s="15">
+        <v>3809</v>
+      </c>
+      <c r="L37" s="1">
+        <v>3284</v>
+      </c>
+      <c r="M37" s="1">
+        <v>4752</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="B38" s="2">
+        <v>242</v>
+      </c>
+      <c r="C38" s="2">
+        <v>9691</v>
+      </c>
+      <c r="D38" s="2">
+        <v>2045</v>
+      </c>
+      <c r="E38" s="2">
+        <v>114</v>
+      </c>
+      <c r="F38" s="2">
+        <v>151</v>
+      </c>
+      <c r="G38" s="2">
+        <v>557</v>
+      </c>
+      <c r="H38" s="2">
+        <v>72</v>
+      </c>
+      <c r="I38" s="2">
+        <v>717</v>
+      </c>
+      <c r="J38" s="2">
+        <v>848</v>
+      </c>
+      <c r="K38" s="16">
         <v>7</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="L38" s="2">
+        <v>1299</v>
+      </c>
+      <c r="M38" s="2">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="B39" s="5">
+        <v>386</v>
+      </c>
+      <c r="C39" s="5">
+        <v>5758</v>
+      </c>
+      <c r="D39" s="5">
+        <v>713</v>
+      </c>
+      <c r="E39" s="5">
+        <v>738</v>
+      </c>
+      <c r="F39" s="5">
+        <v>23</v>
+      </c>
+      <c r="G39" s="5">
+        <v>1683</v>
+      </c>
+      <c r="H39" s="5">
+        <v>64</v>
+      </c>
+      <c r="I39" s="5">
+        <v>578</v>
+      </c>
+      <c r="J39" s="5">
+        <v>2123</v>
+      </c>
+      <c r="K39" s="19">
+        <v>60</v>
+      </c>
+      <c r="L39" s="5">
+        <v>427</v>
+      </c>
+      <c r="M39" s="5">
+        <v>1309</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="B40" s="5">
+        <v>257</v>
+      </c>
+      <c r="C40" s="5">
+        <v>11702</v>
+      </c>
+      <c r="D40" s="5">
+        <v>647</v>
+      </c>
+      <c r="E40" s="5">
+        <v>277</v>
+      </c>
+      <c r="F40" s="5">
+        <v>0</v>
+      </c>
+      <c r="G40" s="5">
+        <v>1</v>
+      </c>
+      <c r="H40" s="5">
+        <v>98</v>
+      </c>
+      <c r="I40" s="5">
+        <v>108</v>
+      </c>
+      <c r="J40" s="5">
+        <v>3921</v>
+      </c>
+      <c r="K40" s="19">
+        <v>73</v>
+      </c>
+      <c r="L40" s="5">
+        <v>530</v>
+      </c>
+      <c r="M40" s="5">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="B41" s="5">
+        <v>586</v>
+      </c>
+      <c r="C41" s="5">
+        <v>18383</v>
+      </c>
+      <c r="D41" s="5">
+        <v>372</v>
+      </c>
+      <c r="E41" s="5">
+        <v>2728</v>
+      </c>
+      <c r="F41" s="5">
+        <v>20</v>
+      </c>
+      <c r="G41" s="5">
+        <v>25</v>
+      </c>
+      <c r="H41" s="5">
+        <v>243</v>
+      </c>
+      <c r="I41" s="5">
+        <v>76</v>
+      </c>
+      <c r="J41" s="5">
+        <v>16624</v>
+      </c>
+      <c r="K41" s="19">
+        <v>63</v>
+      </c>
+      <c r="L41" s="5">
+        <v>335</v>
+      </c>
+      <c r="M41" s="5">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="B42" s="5">
+        <v>307</v>
+      </c>
+      <c r="C42" s="5">
+        <v>3599</v>
+      </c>
+      <c r="D42" s="5">
+        <v>169</v>
+      </c>
+      <c r="E42" s="5">
+        <v>27</v>
+      </c>
+      <c r="F42" s="5">
+        <v>0</v>
+      </c>
+      <c r="G42" s="5">
+        <v>0</v>
+      </c>
+      <c r="H42" s="5">
+        <v>97</v>
+      </c>
+      <c r="I42" s="5">
+        <v>346</v>
+      </c>
+      <c r="J42" s="5">
+        <v>51</v>
+      </c>
+      <c r="K42" s="19">
+        <v>13</v>
+      </c>
+      <c r="L42" s="5">
+        <v>162</v>
+      </c>
+      <c r="M42" s="5">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="B43" s="5">
+        <v>235</v>
+      </c>
+      <c r="C43" s="5">
+        <v>4823</v>
+      </c>
+      <c r="D43" s="5">
+        <v>60</v>
+      </c>
+      <c r="E43" s="5">
+        <v>34</v>
+      </c>
+      <c r="F43" s="5">
+        <v>0</v>
+      </c>
+      <c r="G43" s="5">
+        <v>0</v>
+      </c>
+      <c r="H43" s="5">
+        <v>118</v>
+      </c>
+      <c r="I43" s="5">
+        <v>13</v>
+      </c>
+      <c r="J43" s="5">
+        <v>1428</v>
+      </c>
+      <c r="K43" s="19">
+        <v>0</v>
+      </c>
+      <c r="L43" s="5">
+        <v>71</v>
+      </c>
+      <c r="M43" s="5">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="B44" s="2">
+        <v>211</v>
+      </c>
+      <c r="C44" s="2">
+        <v>13147</v>
+      </c>
+      <c r="D44" s="2">
+        <v>82</v>
+      </c>
+      <c r="E44" s="2">
+        <v>49</v>
+      </c>
+      <c r="F44" s="2">
+        <v>54</v>
+      </c>
+      <c r="G44" s="2">
+        <v>82</v>
+      </c>
+      <c r="H44" s="2">
+        <v>210</v>
+      </c>
+      <c r="I44" s="2">
+        <v>643</v>
+      </c>
+      <c r="J44" s="2">
+        <v>2744</v>
+      </c>
+      <c r="K44" s="16">
+        <v>27</v>
+      </c>
+      <c r="L44" s="2">
+        <v>249</v>
+      </c>
+      <c r="M44" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="B45" s="1">
+        <v>242</v>
+      </c>
+      <c r="C45" s="1">
+        <v>5887</v>
+      </c>
+      <c r="D45" s="1">
+        <v>242</v>
+      </c>
+      <c r="E45" s="1">
+        <v>260</v>
+      </c>
+      <c r="F45" s="1">
+        <v>60</v>
+      </c>
+      <c r="G45" s="1">
+        <v>2065</v>
+      </c>
+      <c r="H45" s="1">
+        <v>69</v>
+      </c>
+      <c r="I45" s="1">
+        <v>1793</v>
+      </c>
+      <c r="J45" s="1">
+        <v>1747</v>
+      </c>
+      <c r="K45" s="15">
+        <v>1781</v>
+      </c>
+      <c r="L45" s="1">
+        <v>1543</v>
+      </c>
+      <c r="M45" s="1">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="B46" s="2">
+        <v>1326</v>
+      </c>
+      <c r="C46" s="2">
+        <v>11524</v>
+      </c>
+      <c r="D46" s="2">
+        <v>627</v>
+      </c>
+      <c r="E46" s="2">
+        <v>332</v>
+      </c>
+      <c r="F46" s="2">
+        <v>373</v>
+      </c>
+      <c r="G46" s="2">
+        <v>3558</v>
+      </c>
+      <c r="H46" s="2">
+        <v>52</v>
+      </c>
+      <c r="I46" s="2">
+        <v>10107</v>
+      </c>
+      <c r="J46" s="2">
+        <v>9883</v>
+      </c>
+      <c r="K46" s="16">
+        <v>478</v>
+      </c>
+      <c r="L46" s="2">
+        <v>5365</v>
+      </c>
+      <c r="M46" s="2">
+        <v>3905</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="B47" s="1">
+        <v>1958</v>
+      </c>
+      <c r="C47" s="1">
+        <v>26925</v>
+      </c>
+      <c r="D47" s="1">
+        <v>1604</v>
+      </c>
+      <c r="E47" s="1">
+        <v>2560</v>
+      </c>
+      <c r="F47" s="1">
+        <v>1358</v>
+      </c>
+      <c r="G47" s="1">
+        <v>1939</v>
+      </c>
+      <c r="H47" s="1">
+        <v>732</v>
+      </c>
+      <c r="I47" s="1">
+        <v>12891</v>
+      </c>
+      <c r="J47" s="1">
+        <v>35108</v>
+      </c>
+      <c r="K47" s="15">
+        <v>1217</v>
+      </c>
+      <c r="L47" s="1">
+        <v>5217</v>
+      </c>
+      <c r="M47" s="1">
+        <v>7412</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="B48" s="2">
+        <v>1641</v>
+      </c>
+      <c r="C48" s="2">
+        <v>17738</v>
+      </c>
+      <c r="D48" s="2">
+        <v>675</v>
+      </c>
+      <c r="E48" s="2">
+        <v>613</v>
+      </c>
+      <c r="F48" s="2">
+        <v>1565</v>
+      </c>
+      <c r="G48" s="2">
+        <v>3533</v>
+      </c>
+      <c r="H48" s="2">
+        <v>17</v>
+      </c>
+      <c r="I48" s="2">
+        <v>9122</v>
+      </c>
+      <c r="J48" s="2">
+        <v>14136</v>
+      </c>
+      <c r="K48" s="16">
+        <v>37</v>
+      </c>
+      <c r="L48" s="2">
+        <v>5449</v>
+      </c>
+      <c r="M48" s="2">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="B49" s="1">
+        <v>1083</v>
+      </c>
+      <c r="C49" s="1">
+        <v>8869</v>
+      </c>
+      <c r="D49" s="1">
+        <v>812</v>
+      </c>
+      <c r="E49" s="1">
+        <v>537</v>
+      </c>
+      <c r="F49" s="1">
+        <v>184</v>
+      </c>
+      <c r="G49" s="1">
+        <v>1327</v>
+      </c>
+      <c r="H49" s="1">
+        <v>778</v>
+      </c>
+      <c r="I49" s="1">
+        <v>5785</v>
+      </c>
+      <c r="J49" s="1">
+        <v>11235</v>
+      </c>
+      <c r="K49" s="15">
+        <v>988</v>
+      </c>
+      <c r="L49" s="1">
+        <v>1670</v>
+      </c>
+      <c r="M49" s="1">
+        <v>3142</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="B50" s="2">
+        <v>4839</v>
+      </c>
+      <c r="C50" s="2">
+        <v>22067</v>
+      </c>
+      <c r="D50" s="2">
+        <v>2973</v>
+      </c>
+      <c r="E50" s="2">
+        <v>2342</v>
+      </c>
+      <c r="F50" s="2">
+        <v>1299</v>
+      </c>
+      <c r="G50" s="2">
+        <v>2592</v>
+      </c>
+      <c r="H50" s="2">
+        <v>662</v>
+      </c>
+      <c r="I50" s="2">
+        <v>18075</v>
+      </c>
+      <c r="J50" s="2">
+        <v>24148</v>
+      </c>
+      <c r="K50" s="16">
+        <v>3986</v>
+      </c>
+      <c r="L50" s="2">
+        <v>4746</v>
+      </c>
+      <c r="M50" s="2">
+        <v>5682</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="B51" s="1">
+        <v>582</v>
+      </c>
+      <c r="C51" s="1">
+        <v>8727</v>
+      </c>
+      <c r="D51" s="1">
+        <v>428</v>
+      </c>
+      <c r="E51" s="1">
+        <v>457</v>
+      </c>
+      <c r="F51" s="1">
+        <v>132</v>
+      </c>
+      <c r="G51" s="1">
+        <v>1760</v>
+      </c>
+      <c r="H51" s="1">
+        <v>74</v>
+      </c>
+      <c r="I51" s="1">
+        <v>3843</v>
+      </c>
+      <c r="J51" s="1">
+        <v>2728</v>
+      </c>
+      <c r="K51" s="15">
+        <v>21</v>
+      </c>
+      <c r="L51" s="1">
+        <v>778</v>
+      </c>
+      <c r="M51" s="1">
+        <v>1489</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="B52" s="2">
+        <v>1162</v>
+      </c>
+      <c r="C52" s="2">
+        <v>18917</v>
+      </c>
+      <c r="D52" s="2">
+        <v>853</v>
+      </c>
+      <c r="E52" s="2">
+        <v>507</v>
+      </c>
+      <c r="F52" s="2">
+        <v>415</v>
+      </c>
+      <c r="G52" s="2">
+        <v>2919</v>
+      </c>
+      <c r="H52" s="2">
+        <v>581</v>
+      </c>
+      <c r="I52" s="2">
+        <v>8370</v>
+      </c>
+      <c r="J52" s="2">
+        <v>13427</v>
+      </c>
+      <c r="K52" s="16">
+        <v>1221</v>
+      </c>
+      <c r="L52" s="2">
+        <v>4709</v>
+      </c>
+      <c r="M52" s="2">
+        <v>3809</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B53" s="1">
+        <v>341</v>
+      </c>
+      <c r="C53" s="1">
+        <v>8918</v>
+      </c>
+      <c r="D53" s="1">
+        <v>449</v>
+      </c>
+      <c r="E53" s="1">
+        <v>313</v>
+      </c>
+      <c r="F53" s="1">
+        <v>409</v>
+      </c>
+      <c r="G53" s="1">
+        <v>1359</v>
+      </c>
+      <c r="H53" s="1">
+        <v>176</v>
+      </c>
+      <c r="I53" s="1">
+        <v>2510</v>
+      </c>
+      <c r="J53" s="1">
+        <v>1041</v>
+      </c>
+      <c r="K53" s="15">
+        <v>74</v>
+      </c>
+      <c r="L53" s="1">
+        <v>1239</v>
+      </c>
+      <c r="M53" s="1">
+        <v>1802</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="B54" s="2">
+        <v>658</v>
+      </c>
+      <c r="C54" s="2">
+        <v>11733</v>
+      </c>
+      <c r="D54" s="2">
+        <v>776</v>
+      </c>
+      <c r="E54" s="2">
+        <v>537</v>
+      </c>
+      <c r="F54" s="2">
+        <v>129</v>
+      </c>
+      <c r="G54" s="2">
+        <v>2044</v>
+      </c>
+      <c r="H54" s="2">
+        <v>73</v>
+      </c>
+      <c r="I54" s="2">
+        <v>1222</v>
+      </c>
+      <c r="J54" s="2">
+        <v>2162</v>
+      </c>
+      <c r="K54" s="16">
+        <v>17</v>
+      </c>
+      <c r="L54" s="2">
+        <v>2240</v>
+      </c>
+      <c r="M54" s="2">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="B55" s="1">
+        <v>742</v>
+      </c>
+      <c r="C55" s="1">
+        <v>12781</v>
+      </c>
+      <c r="D55" s="1">
+        <v>633</v>
+      </c>
+      <c r="E55" s="1">
+        <v>4261</v>
+      </c>
+      <c r="F55" s="1">
+        <v>127</v>
+      </c>
+      <c r="G55" s="1">
+        <v>1362</v>
+      </c>
+      <c r="H55" s="1">
+        <v>93</v>
+      </c>
+      <c r="I55" s="1">
+        <v>2786</v>
+      </c>
+      <c r="J55" s="1">
+        <v>2439</v>
+      </c>
+      <c r="K55" s="15">
         <v>9</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="17"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B16" s="4">
+      <c r="L55" s="1">
+        <v>1735</v>
+      </c>
+      <c r="M55" s="1">
+        <v>1660</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56" s="22" t="s">
+        <v>160</v>
+      </c>
+      <c r="B56" s="22">
         <f>SUM(B12:B15)</f>
-        <v>0</v>
-      </c>
-      <c r="C16" s="4">
-        <f t="shared" ref="C16:M16" si="0">SUM(C12:C15)</f>
-        <v>0</v>
-      </c>
-      <c r="D16" s="4">
+        <v>2263</v>
+      </c>
+      <c r="C56" s="22">
+        <f t="shared" ref="C56:M56" si="0">SUM(C12:C15)</f>
+        <v>19372</v>
+      </c>
+      <c r="D56" s="22">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E16" s="4">
+        <v>2275</v>
+      </c>
+      <c r="E56" s="22">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F16" s="4">
+        <v>2429</v>
+      </c>
+      <c r="F56" s="22">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G16" s="4">
+        <v>674</v>
+      </c>
+      <c r="G56" s="22">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H16" s="4">
+        <v>5647</v>
+      </c>
+      <c r="H56" s="22">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I16" s="4">
+        <v>752</v>
+      </c>
+      <c r="I56" s="22">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J16" s="4">
+        <v>11695</v>
+      </c>
+      <c r="J56" s="22">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K16" s="4">
+        <v>8688</v>
+      </c>
+      <c r="K56" s="22">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L16" s="4">
+        <v>2026</v>
+      </c>
+      <c r="L56" s="22">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M16" s="4">
+        <v>8215</v>
+      </c>
+      <c r="M56" s="22">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="16"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="16"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="16"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="16"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="16"/>
-      <c r="L25" s="2"/>
-      <c r="M25" s="2"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="15"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="16"/>
-      <c r="L27" s="2"/>
-      <c r="M27" s="2"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="15"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="16"/>
-      <c r="L29" s="2"/>
-      <c r="M29" s="2"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="15"/>
-      <c r="L30" s="1"/>
-      <c r="M30" s="1"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="16"/>
-      <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-      <c r="K32" s="15"/>
-      <c r="L32" s="1"/>
-      <c r="M32" s="1"/>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="16"/>
-      <c r="L33" s="2"/>
-      <c r="M33" s="2"/>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="15"/>
-      <c r="L34" s="1"/>
-      <c r="M34" s="1"/>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-      <c r="K35" s="16"/>
-      <c r="L35" s="2"/>
-      <c r="M35" s="2"/>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
-      <c r="K36" s="15"/>
-      <c r="L36" s="1"/>
-      <c r="M36" s="1"/>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
-      <c r="K37" s="16"/>
-      <c r="L37" s="2"/>
-      <c r="M37" s="2"/>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-      <c r="K38" s="15"/>
-      <c r="L38" s="1"/>
-      <c r="M38" s="1"/>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
-      <c r="J39" s="2"/>
-      <c r="K39" s="16"/>
-      <c r="L39" s="2"/>
-      <c r="M39" s="2"/>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B40" s="5"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5"/>
-      <c r="H40" s="5"/>
-      <c r="I40" s="5"/>
-      <c r="J40" s="5"/>
-      <c r="K40" s="19"/>
-      <c r="L40" s="5"/>
-      <c r="M40" s="5"/>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
-      <c r="H41" s="5"/>
-      <c r="I41" s="5"/>
-      <c r="J41" s="5"/>
-      <c r="K41" s="19"/>
-      <c r="L41" s="5"/>
-      <c r="M41" s="5"/>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
-      <c r="G42" s="5"/>
-      <c r="H42" s="5"/>
-      <c r="I42" s="5"/>
-      <c r="J42" s="5"/>
-      <c r="K42" s="19"/>
-      <c r="L42" s="5"/>
-      <c r="M42" s="5"/>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
-      <c r="G43" s="5"/>
-      <c r="H43" s="5"/>
-      <c r="I43" s="5"/>
-      <c r="J43" s="5"/>
-      <c r="K43" s="19"/>
-      <c r="L43" s="5"/>
-      <c r="M43" s="5"/>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
-      <c r="G44" s="5"/>
-      <c r="H44" s="5"/>
-      <c r="I44" s="5"/>
-      <c r="J44" s="5"/>
-      <c r="K44" s="19"/>
-      <c r="L44" s="5"/>
-      <c r="M44" s="5"/>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A45" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B45" s="6">
-        <f>SUM(B40:B44)</f>
-        <v>0</v>
-      </c>
-      <c r="C45" s="6">
-        <f t="shared" ref="C45:M45" si="1">SUM(C40:C44)</f>
-        <v>0</v>
-      </c>
-      <c r="D45" s="6">
+        <v>4332</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A57" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="B57" s="24">
+        <f>SUM(B39:B43)</f>
+        <v>1771</v>
+      </c>
+      <c r="C57" s="24">
+        <f t="shared" ref="C57:M57" si="1">SUM(C39:C43)</f>
+        <v>44265</v>
+      </c>
+      <c r="D57" s="24">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E45" s="6">
+        <v>1961</v>
+      </c>
+      <c r="E57" s="24">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F45" s="6">
+        <v>3804</v>
+      </c>
+      <c r="F57" s="24">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G45" s="6">
+        <v>43</v>
+      </c>
+      <c r="G57" s="24">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H45" s="6">
+        <v>1709</v>
+      </c>
+      <c r="H57" s="24">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I45" s="6">
+        <v>620</v>
+      </c>
+      <c r="I57" s="24">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J45" s="6">
+        <v>1121</v>
+      </c>
+      <c r="J57" s="24">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K45" s="6">
+        <v>24147</v>
+      </c>
+      <c r="K57" s="24">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L45" s="6">
+        <v>209</v>
+      </c>
+      <c r="L57" s="24">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M45" s="6">
+        <v>1525</v>
+      </c>
+      <c r="M57" s="24">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
-      <c r="H46" s="2"/>
-      <c r="I46" s="2"/>
-      <c r="J46" s="2"/>
-      <c r="K46" s="16"/>
-      <c r="L46" s="2"/>
-      <c r="M46" s="2"/>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
-      <c r="I47" s="1"/>
-      <c r="J47" s="1"/>
-      <c r="K47" s="15"/>
-      <c r="L47" s="1"/>
-      <c r="M47" s="1"/>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
-      <c r="E48" s="2"/>
-      <c r="F48" s="2"/>
-      <c r="G48" s="2"/>
-      <c r="H48" s="2"/>
-      <c r="I48" s="2"/>
-      <c r="J48" s="2"/>
-      <c r="K48" s="16"/>
-      <c r="L48" s="2"/>
-      <c r="M48" s="2"/>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
-      <c r="I49" s="1"/>
-      <c r="J49" s="1"/>
-      <c r="K49" s="15"/>
-      <c r="L49" s="1"/>
-      <c r="M49" s="1"/>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2"/>
-      <c r="F50" s="2"/>
-      <c r="G50" s="2"/>
-      <c r="H50" s="2"/>
-      <c r="I50" s="2"/>
-      <c r="J50" s="2"/>
-      <c r="K50" s="16"/>
-      <c r="L50" s="2"/>
-      <c r="M50" s="2"/>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
-      <c r="H51" s="1"/>
-      <c r="I51" s="1"/>
-      <c r="J51" s="1"/>
-      <c r="K51" s="15"/>
-      <c r="L51" s="1"/>
-      <c r="M51" s="1"/>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B52" s="2"/>
-      <c r="C52" s="2"/>
-      <c r="D52" s="2"/>
-      <c r="E52" s="2"/>
-      <c r="F52" s="2"/>
-      <c r="G52" s="2"/>
-      <c r="H52" s="2"/>
-      <c r="I52" s="2"/>
-      <c r="J52" s="2"/>
-      <c r="K52" s="16"/>
-      <c r="L52" s="2"/>
-      <c r="M52" s="2"/>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
-      <c r="I53" s="1"/>
-      <c r="J53" s="1"/>
-      <c r="K53" s="15"/>
-      <c r="L53" s="1"/>
-      <c r="M53" s="1"/>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
-      <c r="E54" s="2"/>
-      <c r="F54" s="2"/>
-      <c r="G54" s="2"/>
-      <c r="H54" s="2"/>
-      <c r="I54" s="2"/>
-      <c r="J54" s="2"/>
-      <c r="K54" s="16"/>
-      <c r="L54" s="2"/>
-      <c r="M54" s="2"/>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
-      <c r="G55" s="1"/>
-      <c r="H55" s="1"/>
-      <c r="I55" s="1"/>
-      <c r="J55" s="1"/>
-      <c r="K55" s="15"/>
-      <c r="L55" s="1"/>
-      <c r="M55" s="1"/>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
-      <c r="D56" s="2"/>
-      <c r="E56" s="2"/>
-      <c r="F56" s="2"/>
-      <c r="G56" s="2"/>
-      <c r="H56" s="2"/>
-      <c r="I56" s="2"/>
-      <c r="J56" s="2"/>
-      <c r="K56" s="16"/>
-      <c r="L56" s="2"/>
-      <c r="M56" s="2"/>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
-      <c r="E57" s="1"/>
-      <c r="F57" s="1"/>
-      <c r="G57" s="1"/>
-      <c r="H57" s="1"/>
-      <c r="I57" s="1"/>
-      <c r="J57" s="1"/>
-      <c r="K57" s="15"/>
-      <c r="L57" s="1"/>
-      <c r="M57" s="1"/>
+        <v>2099</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A58" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="B58" s="23">
+        <f>SUM(B2:B55)</f>
+        <v>108652</v>
+      </c>
+      <c r="C58" s="23">
+        <f t="shared" ref="C58:M58" si="2">SUM(C2:C55)</f>
+        <v>829620</v>
+      </c>
+      <c r="D58" s="23">
+        <f t="shared" si="2"/>
+        <v>59052</v>
+      </c>
+      <c r="E58" s="23">
+        <f t="shared" si="2"/>
+        <v>64833</v>
+      </c>
+      <c r="F58" s="23">
+        <f t="shared" si="2"/>
+        <v>35511</v>
+      </c>
+      <c r="G58" s="23">
+        <f t="shared" si="2"/>
+        <v>117743</v>
+      </c>
+      <c r="H58" s="23">
+        <f t="shared" si="2"/>
+        <v>28295</v>
+      </c>
+      <c r="I58" s="23">
+        <f t="shared" si="2"/>
+        <v>457234</v>
+      </c>
+      <c r="J58" s="23">
+        <f t="shared" si="2"/>
+        <v>573667</v>
+      </c>
+      <c r="K58" s="23">
+        <f t="shared" si="2"/>
+        <v>42383</v>
+      </c>
+      <c r="L58" s="23">
+        <f t="shared" si="2"/>
+        <v>161928</v>
+      </c>
+      <c r="M58" s="23">
+        <f t="shared" si="2"/>
+        <v>152373</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M57" xr:uid="{0334C0AC-E6B4-49E4-BF68-7AE53436DE88}"/>
+  <autoFilter ref="A1:M55" xr:uid="{0334C0AC-E6B4-49E4-BF68-7AE53436DE88}"/>
+  <dataValidations count="3">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Based on the monthly circulation spreadsheet as run on January 1, 2023 and throughout 2022" sqref="B1 L1 M1" xr:uid="{9AFE055E-223F-49E5-9C15-AE657F748B31}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Data from report 3695 as run on January 1, 2023" sqref="C1 D1 E1 F1 G1 H1" xr:uid="{1EFFAEFB-4390-4A7E-8AA3-939BCB186794}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Based on circulation by item type spreadsheet as run on January 1, 2023 and throughout 2022" sqref="I1 J1 K1" xr:uid="{DC9878E4-99C7-499B-89ED-4FF62F916377}"/>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80613C6A-86D2-4637-A1C1-305CDD262B00}">
-  <dimension ref="A1:M57"/>
+  <dimension ref="A1:N57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2386,48 +3933,51 @@
     <col min="1" max="13" width="16.7109375" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="9" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:14" s="9" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="11" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N1" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -2467,9 +4017,12 @@
       <c r="M2" s="1">
         <v>11045</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="N2" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2">
@@ -2508,8 +4061,11 @@
       <c r="M3" s="2">
         <v>4626</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N3" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -2549,9 +4105,12 @@
       <c r="M4" s="1">
         <v>11295</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="N4" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2">
@@ -2590,8 +4149,11 @@
       <c r="M5" s="2">
         <v>242</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N5" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -2631,9 +4193,12 @@
       <c r="M6" s="1">
         <v>11500</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="N6" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="2">
@@ -2672,8 +4237,11 @@
       <c r="M7" s="2">
         <v>1713</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N7" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -2713,9 +4281,12 @@
       <c r="M8" s="1">
         <v>1105</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="N8" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="2">
@@ -2754,8 +4325,11 @@
       <c r="M9" s="2">
         <v>152</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N9" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -2795,9 +4369,12 @@
       <c r="M10" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="N10" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="2">
@@ -2836,8 +4413,11 @@
       <c r="M11" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N11" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
@@ -2877,8 +4457,11 @@
       <c r="M12" s="3">
         <v>475</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N12" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
@@ -2918,8 +4501,11 @@
       <c r="M13" s="3">
         <v>1786</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N13" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
@@ -2959,8 +4545,11 @@
       <c r="M14" s="3">
         <v>1731</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N14" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
@@ -3000,8 +4589,11 @@
       <c r="M15" s="3">
         <v>1278</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N15" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>54</v>
       </c>
@@ -3047,9 +4639,12 @@
       <c r="M16" s="4">
         <v>5270</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="N16" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="2">
@@ -3088,8 +4683,11 @@
       <c r="M17" s="2">
         <v>300</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N17" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -3129,9 +4727,12 @@
       <c r="M18" s="1">
         <v>5518</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="N18" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="2">
@@ -3170,8 +4771,11 @@
       <c r="M19" s="2">
         <v>816</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N19" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -3211,9 +4815,12 @@
       <c r="M20" s="1">
         <v>4671</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="N20" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
         <v>79</v>
       </c>
       <c r="B21" s="2">
@@ -3252,8 +4859,11 @@
       <c r="M21" s="2">
         <v>33</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N21" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
@@ -3293,9 +4903,12 @@
       <c r="M22" s="1">
         <v>4568</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="N22" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
         <v>20</v>
       </c>
       <c r="B23" s="2">
@@ -3334,8 +4947,11 @@
       <c r="M23" s="2">
         <v>306</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N23" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
@@ -3375,9 +4991,12 @@
       <c r="M24" s="1">
         <v>5143</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="N24" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="14" t="s">
         <v>22</v>
       </c>
       <c r="B25" s="2">
@@ -3416,8 +5035,11 @@
       <c r="M25" s="2">
         <v>17589</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N25" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
@@ -3457,9 +5079,12 @@
       <c r="M26" s="1">
         <v>1645</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="N26" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="14" t="s">
         <v>24</v>
       </c>
       <c r="B27" s="2">
@@ -3498,8 +5123,11 @@
       <c r="M27" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N27" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
@@ -3539,9 +5167,12 @@
       <c r="M28" s="1">
         <v>2305</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="N28" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="14" t="s">
         <v>26</v>
       </c>
       <c r="B29" s="2">
@@ -3580,8 +5211,11 @@
       <c r="M29" s="2">
         <v>913</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N29" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>27</v>
       </c>
@@ -3621,9 +5255,12 @@
       <c r="M30" s="1">
         <v>3548</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="N30" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="14" t="s">
         <v>28</v>
       </c>
       <c r="B31" s="2">
@@ -3662,8 +5299,11 @@
       <c r="M31" s="2">
         <v>147</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N31" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>29</v>
       </c>
@@ -3703,9 +5343,12 @@
       <c r="M32" s="1">
         <v>496</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+      <c r="N32" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" s="14" t="s">
         <v>30</v>
       </c>
       <c r="B33" s="2">
@@ -3744,8 +5387,11 @@
       <c r="M33" s="2">
         <v>5163</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N33" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>31</v>
       </c>
@@ -3785,9 +5431,12 @@
       <c r="M34" s="1">
         <v>4156</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+      <c r="N34" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35" s="14" t="s">
         <v>32</v>
       </c>
       <c r="B35" s="2">
@@ -3826,8 +5475,11 @@
       <c r="M35" s="2">
         <v>2171</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N35" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>33</v>
       </c>
@@ -3867,9 +5519,12 @@
       <c r="M36" s="1">
         <v>8730</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+      <c r="N36" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" s="14" t="s">
         <v>34</v>
       </c>
       <c r="B37" s="2">
@@ -3908,8 +5563,11 @@
       <c r="M37" s="2">
         <v>2115</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N37" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>35</v>
       </c>
@@ -3949,9 +5607,12 @@
       <c r="M38" s="1">
         <v>3921</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+      <c r="N38" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A39" s="14" t="s">
         <v>36</v>
       </c>
       <c r="B39" s="2">
@@ -3990,8 +5651,11 @@
       <c r="M39" s="2">
         <v>255</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N39" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>37</v>
       </c>
@@ -4031,8 +5695,11 @@
       <c r="M40" s="5">
         <v>239</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N40" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>38</v>
       </c>
@@ -4072,8 +5739,11 @@
       <c r="M41" s="5">
         <v>330</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N41" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>39</v>
       </c>
@@ -4113,8 +5783,11 @@
       <c r="M42" s="5">
         <v>103</v>
       </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N42" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>40</v>
       </c>
@@ -4154,8 +5827,11 @@
       <c r="M43" s="5">
         <v>63</v>
       </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N43" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>41</v>
       </c>
@@ -4195,8 +5871,11 @@
       <c r="M44" s="5">
         <v>123</v>
       </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N44" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>55</v>
       </c>
@@ -4242,9 +5921,12 @@
       <c r="M45" s="6">
         <v>858</v>
       </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
+      <c r="N45" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A46" s="14" t="s">
         <v>42</v>
       </c>
       <c r="B46" s="2">
@@ -4283,8 +5965,11 @@
       <c r="M46" s="2">
         <v>364</v>
       </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N46" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>43</v>
       </c>
@@ -4324,9 +6009,12 @@
       <c r="M47" s="1">
         <v>844</v>
       </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
+      <c r="N47" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A48" s="14" t="s">
         <v>44</v>
       </c>
       <c r="B48" s="2">
@@ -4365,8 +6053,11 @@
       <c r="M48" s="2">
         <v>3833</v>
       </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N48" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>45</v>
       </c>
@@ -4406,9 +6097,12 @@
       <c r="M49" s="1">
         <v>7347</v>
       </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
+      <c r="N49" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A50" s="14" t="s">
         <v>46</v>
       </c>
       <c r="B50" s="2">
@@ -4447,8 +6141,11 @@
       <c r="M50" s="2">
         <v>2038</v>
       </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N50" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>47</v>
       </c>
@@ -4488,9 +6185,12 @@
       <c r="M51" s="1">
         <v>3101</v>
       </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
+      <c r="N51" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A52" s="14" t="s">
         <v>48</v>
       </c>
       <c r="B52" s="2">
@@ -4529,8 +6229,11 @@
       <c r="M52" s="2">
         <v>4939</v>
       </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N52" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>49</v>
       </c>
@@ -4570,9 +6273,12 @@
       <c r="M53" s="1">
         <v>1397</v>
       </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
+      <c r="N53" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A54" s="14" t="s">
         <v>50</v>
       </c>
       <c r="B54" s="2">
@@ -4611,8 +6317,11 @@
       <c r="M54" s="2">
         <v>4195</v>
       </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N54" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>51</v>
       </c>
@@ -4652,9 +6361,12 @@
       <c r="M55" s="1">
         <v>1597</v>
       </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
+      <c r="N55" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A56" s="14" t="s">
         <v>52</v>
       </c>
       <c r="B56" s="2">
@@ -4693,8 +6405,11 @@
       <c r="M56" s="2">
         <v>430</v>
       </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N56" s="11">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>53</v>
       </c>
@@ -4734,10 +6449,13 @@
       <c r="M57" s="1">
         <v>1799</v>
       </c>
+      <c r="N57" s="11">
+        <v>2021</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:M1" xr:uid="{FCBD2F65-B525-414A-B8EE-C184E238B9F1}"/>
-  <dataValidations count="6">
+  <dataValidations disablePrompts="1" count="6">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="New question for 2021 - no data available" sqref="K1" xr:uid="{A363F40A-2D60-4D05-B783-C4A4749E6232}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Based on the monthly circulation spreadsheet" sqref="I1:J1 B1" xr:uid="{C7E2BA89-70A9-4ADB-9611-4A08D12539F6}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Counts the number of Next items your library received from  other Next libraries during the month - regardless of whether or not the patron who requested the item actually checked it out or not." sqref="L1" xr:uid="{B3A8708B-ECC4-485B-B1EE-0B7548896D7A}"/>
@@ -4754,10 +6472,10 @@
   <dimension ref="A1:O57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="O1" sqref="O1:O57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>